<commit_message>
Changed rankby to prominence
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -57,13 +57,13 @@
     <t>Group by coordinates</t>
   </si>
   <si>
-    <t>Generate dot product matrix</t>
-  </si>
-  <si>
     <t>Convolve</t>
   </si>
   <si>
-    <t>Ploting</t>
+    <t>Generate matrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dot product logic </t>
   </si>
 </sst>
 </file>
@@ -434,7 +434,7 @@
   <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -507,15 +507,15 @@
       </c>
       <c r="I2" s="2">
         <f>SUM(C1:C99)/60</f>
-        <v>0.63333333333333441</v>
+        <v>1.9333333333333336</v>
       </c>
       <c r="J2" s="2">
         <f>H2*AVERAGE(F1:F99)</f>
-        <v>3.4833333333333392</v>
+        <v>3.2236111111111132</v>
       </c>
       <c r="K2" s="2">
         <f>J2-I2</f>
-        <v>2.850000000000005</v>
+        <v>1.2902777777777796</v>
       </c>
       <c r="M2" s="12"/>
       <c r="N2" s="1"/>
@@ -557,11 +557,20 @@
       <c r="B4" s="9">
         <v>30</v>
       </c>
+      <c r="C4" s="2">
+        <f>(E4-D4)*1440</f>
+        <v>37.999999999999943</v>
+      </c>
       <c r="D4" s="8">
         <v>0.25555555555555559</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="9"/>
+      <c r="E4" s="14">
+        <v>0.28194444444444444</v>
+      </c>
+      <c r="F4" s="9">
+        <f>C4/B4</f>
+        <v>1.2666666666666648</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="7"/>
       <c r="I4" s="1"/>
@@ -572,14 +581,25 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="6">
-        <v>30</v>
-      </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
+        <v>45</v>
+      </c>
+      <c r="C5" s="2">
+        <f>(E5-D5)*1440</f>
+        <v>40.000000000000014</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0.28472222222222221</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0.3125</v>
+      </c>
+      <c r="F5" s="9">
+        <f>C5/B5</f>
+        <v>0.88888888888888917</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="7"/>
       <c r="I5" s="1"/>
@@ -593,9 +613,11 @@
         <v>15</v>
       </c>
       <c r="B6" s="9">
-        <v>15</v>
-      </c>
-      <c r="D6" s="8"/>
+        <v>30</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.34375</v>
+      </c>
       <c r="E6" s="8"/>
       <c r="F6" s="9"/>
       <c r="G6" s="1"/>
@@ -606,10 +628,10 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="6">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="8"/>

</xml_diff>

<commit_message>
Graph plotting and dot product
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -434,7 +434,7 @@
   <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -507,15 +507,15 @@
       </c>
       <c r="I2" s="2">
         <f>SUM(C1:C99)/60</f>
-        <v>1.9333333333333336</v>
+        <v>2.3833333333333333</v>
       </c>
       <c r="J2" s="2">
         <f>H2*AVERAGE(F1:F99)</f>
-        <v>3.2236111111111132</v>
+        <v>3.0738888888888902</v>
       </c>
       <c r="K2" s="2">
         <f>J2-I2</f>
-        <v>1.2902777777777796</v>
+        <v>0.69055555555555692</v>
       </c>
       <c r="M2" s="12"/>
       <c r="N2" s="1"/>
@@ -615,11 +615,20 @@
       <c r="B6" s="9">
         <v>30</v>
       </c>
+      <c r="C6" s="2">
+        <f>(E6-D6)*1440</f>
+        <v>26.999999999999986</v>
+      </c>
       <c r="D6" s="8">
         <v>0.34375</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9"/>
+      <c r="E6" s="8">
+        <v>0.36249999999999999</v>
+      </c>
+      <c r="F6" s="9">
+        <f>C6/B6</f>
+        <v>0.89999999999999958</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="J6" s="1"/>
       <c r="M6" s="12"/>

</xml_diff>